<commit_message>
Shelly's Access Line Splitter Improvements
</commit_message>
<xml_diff>
--- a/hyperlinker/app/referencesheets/Hotline Para List.xlsx
+++ b/hyperlinker/app/referencesheets/Hotline Para List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackley\Python\GitPython\hyperlinker\app\referencesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1C4D93-03FD-4C08-82CE-F7ABB1955E61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F57D6FD-82C5-41FA-9EDB-BB818F3A3A13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="20010" windowHeight="8025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
-  <si>
-    <t>Morales-Robinson, Ana</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Start Date</t>
   </si>
@@ -37,9 +34,6 @@
     <t>Ikram, Nabah</t>
   </si>
   <si>
-    <t>Suriel, Salatiel</t>
-  </si>
-  <si>
     <t>Paz, Alexis</t>
   </si>
   <si>
@@ -52,12 +46,6 @@
     <t>Navas, Keyra M</t>
   </si>
   <si>
-    <t>Ruiz-Caceres, Gabriela A</t>
-  </si>
-  <si>
-    <t>Dong, Xingyou</t>
-  </si>
-  <si>
     <t>Baldova, Maria</t>
   </si>
   <si>
@@ -119,6 +107,27 @@
   </si>
   <si>
     <t>Rodney, Gabby A</t>
+  </si>
+  <si>
+    <t>Morales-Robinson, Ana Y.</t>
+  </si>
+  <si>
+    <t>Ruiz-Caceres, Gaby A</t>
+  </si>
+  <si>
+    <t>Suriel, Sal</t>
+  </si>
+  <si>
+    <t>Dong, Sean</t>
+  </si>
+  <si>
+    <t>Start Date 2</t>
+  </si>
+  <si>
+    <t>End Date 2</t>
+  </si>
+  <si>
+    <t>Agarwala, Shelly</t>
   </si>
 </sst>
 </file>
@@ -517,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,113 +537,124 @@
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>44410</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1">
         <v>43753</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>43753</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>43753</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
+        <v>40909</v>
+      </c>
+      <c r="C6" s="1">
         <v>43021</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>44268</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>44060</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>44117</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>44130</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
         <v>42044</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>42044</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>42156</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1">
         <v>42490</v>
@@ -643,25 +663,25 @@
         <v>44435</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1">
         <v>42891</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1">
         <v>43080</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>42044</v>
@@ -672,7 +692,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>42042</v>
@@ -683,7 +703,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>42170</v>
@@ -694,7 +714,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>42156</v>
@@ -705,7 +725,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1">
         <v>42255</v>
@@ -716,7 +736,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1">
         <v>42492</v>
@@ -727,7 +747,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1">
         <v>42492</v>
@@ -738,7 +758,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>42562</v>
@@ -749,7 +769,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1">
         <v>43108</v>
@@ -760,7 +780,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1">
         <v>43500</v>
@@ -771,7 +791,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1">
         <v>43668</v>
@@ -782,7 +802,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1">
         <v>42492</v>
@@ -793,7 +813,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1">
         <v>42492</v>
@@ -804,7 +824,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1">
         <v>42492</v>
@@ -815,7 +835,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1">
         <v>42891</v>
@@ -826,13 +846,21 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1">
         <v>42042</v>
       </c>
       <c r="C31" s="1">
         <v>43763</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="1">
+        <v>40909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>